<commit_message>
Adicionando a base para o funcionamento
</commit_message>
<xml_diff>
--- a/Forca/database/palavras.xlsx
+++ b/Forca/database/palavras.xlsx
@@ -1,39 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
-  </bookViews>
+  <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Palavras</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -48,7 +30,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -56,36 +38,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -164,6 +128,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -198,6 +163,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -232,20 +198,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -367,25 +329,75 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:2">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Palavras</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Algo</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Maio</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>